<commit_message>
Add annex case to createDoc util function
</commit_message>
<xml_diff>
--- a/files/input/offersData.xlsx
+++ b/files/input/offersData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="7">
   <si>
     <t>JONESBORO SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>bid</t>
+  </si>
+  <si>
+    <t>nip</t>
   </si>
 </sst>
 </file>
@@ -355,22 +358,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="48.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -378,10 +382,13 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -389,10 +396,13 @@
         <v>0</v>
       </c>
       <c r="C2">
+        <v>5252516964</v>
+      </c>
+      <c r="D2">
         <v>3500</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -400,10 +410,13 @@
         <v>1</v>
       </c>
       <c r="C3">
+        <v>7720100638</v>
+      </c>
+      <c r="D3">
         <v>4000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -411,10 +424,13 @@
         <v>2</v>
       </c>
       <c r="C4">
+        <v>8982126450</v>
+      </c>
+      <c r="D4">
         <v>4500</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -422,10 +438,13 @@
         <v>1</v>
       </c>
       <c r="C5">
+        <v>7720100638</v>
+      </c>
+      <c r="D5">
         <v>3800</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -433,10 +452,13 @@
         <v>2</v>
       </c>
       <c r="C6">
+        <v>8982126450</v>
+      </c>
+      <c r="D6">
         <v>3700</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -444,10 +466,13 @@
         <v>0</v>
       </c>
       <c r="C7">
+        <v>5252516964</v>
+      </c>
+      <c r="D7">
         <v>3200</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -455,10 +480,13 @@
         <v>2</v>
       </c>
       <c r="C8">
+        <v>8982126450</v>
+      </c>
+      <c r="D8">
         <v>3400</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -466,10 +494,13 @@
         <v>0</v>
       </c>
       <c r="C9">
+        <v>5252516964</v>
+      </c>
+      <c r="D9">
         <v>3800</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -477,7 +508,262 @@
         <v>1</v>
       </c>
       <c r="C10">
+        <v>7720100638</v>
+      </c>
+      <c r="D10">
         <v>3900</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>5252516964</v>
+      </c>
+      <c r="D11">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>7720100638</v>
+      </c>
+      <c r="D12">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>5252516964</v>
+      </c>
+      <c r="D13">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>7720100638</v>
+      </c>
+      <c r="D14">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>5252516964</v>
+      </c>
+      <c r="D15">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>7720100638</v>
+      </c>
+      <c r="D16">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>5252516964</v>
+      </c>
+      <c r="D17">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>7720100638</v>
+      </c>
+      <c r="D18">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>5252516964</v>
+      </c>
+      <c r="D19">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>7720100638</v>
+      </c>
+      <c r="D20">
+        <v>5100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>5252516964</v>
+      </c>
+      <c r="D21">
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>7720100638</v>
+      </c>
+      <c r="D22">
+        <v>5300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>7720100638</v>
+      </c>
+      <c r="D23">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>7720100638</v>
+      </c>
+      <c r="D24">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>12</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>7720100638</v>
+      </c>
+      <c r="D25">
+        <v>5600</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>7720100638</v>
+      </c>
+      <c r="D26">
+        <v>5700</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>14</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>7720100638</v>
+      </c>
+      <c r="D27">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>15</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>7720100638</v>
+      </c>
+      <c r="D28">
+        <v>5000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>